<commit_message>
corregido fallo de pipes
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jl_ut\Documents\42Madrid\Minishell_local\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jl_ut\Documents\GitHub\C4_minishell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FADB284-4B60-40A6-A7C4-D61C44732D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CE8DDF-567D-4F04-B113-5E9D5DC970CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="281">
   <si>
     <t>Test</t>
   </si>
@@ -1123,6 +1123,18 @@
       </rPr>
       <t xml:space="preserve">  (status = 0 por grep, que no encuentra nada)</t>
     </r>
+  </si>
+  <si>
+    <t>cat | cat | ls</t>
+  </si>
+  <si>
+    <t>ejecuta ls y sale de edición pulsando dos veces INTRO</t>
+  </si>
+  <si>
+    <t>&lt;&lt; EOF</t>
+  </si>
+  <si>
+    <t>no hace nada al salir de heredoc</t>
   </si>
 </sst>
 </file>
@@ -1661,60 +1673,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1727,6 +1685,60 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -1947,10 +1959,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="150" zoomScaleNormal="150" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="E96" sqref="E96"/>
+    <sheetView tabSelected="1" topLeftCell="B106" zoomScale="150" zoomScaleNormal="150" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="F127" sqref="F127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1984,7 +1996,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="85" t="s">
         <v>91</v>
       </c>
       <c r="B2" s="23" t="s">
@@ -1994,109 +2006,109 @@
         <v>92</v>
       </c>
       <c r="D2" s="38"/>
-      <c r="E2" s="89"/>
+      <c r="E2" s="71"/>
       <c r="F2" s="54" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="78"/>
+      <c r="A3" s="86"/>
       <c r="B3" s="24" t="s">
         <v>223</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="38"/>
-      <c r="E3" s="89"/>
+      <c r="E3" s="71"/>
       <c r="F3" s="54" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="78"/>
+      <c r="A4" s="86"/>
       <c r="B4" s="24" t="s">
         <v>224</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="38"/>
-      <c r="E4" s="89"/>
+      <c r="E4" s="71"/>
       <c r="F4" s="54" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="79"/>
+      <c r="A5" s="87"/>
       <c r="B5" s="23" t="s">
         <v>114</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="38"/>
-      <c r="E5" s="89"/>
+      <c r="E5" s="71"/>
       <c r="F5" s="54" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="79"/>
+      <c r="A6" s="87"/>
       <c r="B6" s="24" t="s">
         <v>225</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="38"/>
-      <c r="E6" s="89"/>
+      <c r="E6" s="71"/>
       <c r="F6" s="54" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="79"/>
+      <c r="A7" s="87"/>
       <c r="B7" s="24" t="s">
         <v>226</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="38"/>
-      <c r="E7" s="89"/>
+      <c r="E7" s="71"/>
       <c r="F7" s="54" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="79"/>
+      <c r="A8" s="87"/>
       <c r="B8" s="25" t="s">
         <v>251</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="38"/>
-      <c r="E8" s="89"/>
+      <c r="E8" s="71"/>
       <c r="F8" s="54" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="79"/>
+      <c r="A9" s="87"/>
       <c r="B9" s="25" t="s">
         <v>225</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="38"/>
-      <c r="E9" s="90"/>
+      <c r="E9" s="72"/>
       <c r="F9" s="54" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="80"/>
+      <c r="A10" s="88"/>
       <c r="B10" s="26" t="s">
         <v>226</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="91"/>
+      <c r="E10" s="73"/>
       <c r="F10" s="55" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="82" t="s">
         <v>227</v>
       </c>
       <c r="B11" s="27" t="s">
@@ -2104,79 +2116,79 @@
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="39"/>
-      <c r="E11" s="92"/>
+      <c r="E11" s="74"/>
       <c r="F11" s="56" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="75"/>
+      <c r="A12" s="83"/>
       <c r="B12" s="28" t="s">
         <v>131</v>
       </c>
       <c r="D12" s="18"/>
-      <c r="E12" s="89"/>
+      <c r="E12" s="71"/>
       <c r="F12" s="54" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="75"/>
+      <c r="A13" s="83"/>
       <c r="B13" s="28" t="s">
         <v>132</v>
       </c>
       <c r="D13" s="18"/>
-      <c r="E13" s="89"/>
+      <c r="E13" s="71"/>
       <c r="F13" s="54" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="75"/>
+      <c r="A14" s="83"/>
       <c r="B14" s="25" t="s">
         <v>124</v>
       </c>
       <c r="D14" s="18"/>
-      <c r="E14" s="89"/>
+      <c r="E14" s="71"/>
       <c r="F14" s="54" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="75"/>
+      <c r="A15" s="83"/>
       <c r="B15" s="25" t="s">
         <v>125</v>
       </c>
       <c r="D15" s="18"/>
-      <c r="E15" s="89"/>
+      <c r="E15" s="71"/>
       <c r="F15" s="54" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="75"/>
+      <c r="A16" s="83"/>
       <c r="B16" s="25" t="s">
         <v>153</v>
       </c>
       <c r="D16" s="18"/>
-      <c r="E16" s="89"/>
+      <c r="E16" s="71"/>
       <c r="F16" s="54" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="75"/>
+      <c r="A17" s="83"/>
       <c r="B17" s="25" t="s">
         <v>154</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="89"/>
+      <c r="E17" s="71"/>
       <c r="F17" s="57" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="75"/>
+      <c r="A18" s="83"/>
       <c r="B18" s="28" t="s">
         <v>177</v>
       </c>
@@ -2189,79 +2201,79 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="75"/>
+      <c r="A19" s="83"/>
       <c r="B19" s="23" t="s">
         <v>118</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="38"/>
-      <c r="E19" s="90"/>
+      <c r="E19" s="72"/>
       <c r="F19" s="58" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="75"/>
+      <c r="A20" s="83"/>
       <c r="B20" s="23" t="s">
         <v>111</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="38"/>
-      <c r="E20" s="89"/>
+      <c r="E20" s="71"/>
       <c r="F20" s="54" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="75"/>
+      <c r="A21" s="83"/>
       <c r="B21" s="23" t="s">
         <v>106</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="40"/>
-      <c r="E21" s="89"/>
+      <c r="E21" s="71"/>
       <c r="F21" s="54" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="75"/>
+      <c r="A22" s="83"/>
       <c r="B22" s="23" t="s">
         <v>95</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="40"/>
-      <c r="E22" s="89"/>
+      <c r="E22" s="71"/>
       <c r="F22" s="54" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="75"/>
+      <c r="A23" s="83"/>
       <c r="B23" s="24" t="s">
         <v>266</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="40"/>
-      <c r="E23" s="89"/>
+      <c r="E23" s="71"/>
       <c r="F23" s="54" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="75"/>
+      <c r="A24" s="83"/>
       <c r="B24" s="24" t="s">
         <v>265</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="40"/>
-      <c r="E24" s="89"/>
+      <c r="E24" s="71"/>
       <c r="F24" s="54" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="75"/>
+      <c r="A25" s="83"/>
       <c r="B25" s="29" t="s">
         <v>166</v>
       </c>
@@ -2269,13 +2281,13 @@
         <v>93</v>
       </c>
       <c r="D25" s="41"/>
-      <c r="E25" s="89"/>
+      <c r="E25" s="71"/>
       <c r="F25" s="59" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="82" t="s">
         <v>94</v>
       </c>
       <c r="B26" s="24" t="s">
@@ -2283,13 +2295,13 @@
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="42"/>
-      <c r="E26" s="92"/>
+      <c r="E26" s="74"/>
       <c r="F26" s="60" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="76"/>
+      <c r="A27" s="84"/>
       <c r="B27" s="30" t="s">
         <v>243</v>
       </c>
@@ -2297,13 +2309,13 @@
         <v>0</v>
       </c>
       <c r="D27" s="41"/>
-      <c r="E27" s="91"/>
+      <c r="E27" s="73"/>
       <c r="F27" s="61" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="84" t="s">
+      <c r="A28" s="92" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="24" t="s">
@@ -2313,25 +2325,25 @@
         <v>4</v>
       </c>
       <c r="D28" s="38"/>
-      <c r="E28" s="89"/>
+      <c r="E28" s="71"/>
       <c r="F28" s="54" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="84"/>
+      <c r="A29" s="92"/>
       <c r="B29" s="24" t="s">
         <v>126</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="38"/>
-      <c r="E29" s="89"/>
+      <c r="E29" s="71"/>
       <c r="F29" s="62" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="84"/>
+      <c r="A30" s="92"/>
       <c r="B30" s="24" t="s">
         <v>5</v>
       </c>
@@ -2339,13 +2351,13 @@
         <v>4</v>
       </c>
       <c r="D30" s="38"/>
-      <c r="E30" s="89"/>
+      <c r="E30" s="71"/>
       <c r="F30" s="54" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="84"/>
+      <c r="A31" s="92"/>
       <c r="B31" s="24" t="s">
         <v>6</v>
       </c>
@@ -2353,13 +2365,13 @@
         <v>7</v>
       </c>
       <c r="D31" s="38"/>
-      <c r="E31" s="89"/>
+      <c r="E31" s="71"/>
       <c r="F31" s="54" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="84"/>
+      <c r="A32" s="92"/>
       <c r="B32" s="24" t="s">
         <v>8</v>
       </c>
@@ -2367,7 +2379,7 @@
         <v>9</v>
       </c>
       <c r="D32" s="38"/>
-      <c r="E32" s="93" t="s">
+      <c r="E32" s="75" t="s">
         <v>253</v>
       </c>
       <c r="F32" s="54" t="s">
@@ -2375,7 +2387,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="84"/>
+      <c r="A33" s="92"/>
       <c r="B33" s="24" t="s">
         <v>10</v>
       </c>
@@ -2383,13 +2395,13 @@
         <v>11</v>
       </c>
       <c r="D33" s="38"/>
-      <c r="E33" s="89"/>
+      <c r="E33" s="71"/>
       <c r="F33" s="63" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="84"/>
+      <c r="A34" s="92"/>
       <c r="B34" s="24" t="s">
         <v>12</v>
       </c>
@@ -2397,13 +2409,13 @@
         <v>13</v>
       </c>
       <c r="D34" s="38"/>
-      <c r="E34" s="89"/>
+      <c r="E34" s="71"/>
       <c r="F34" s="54" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="84"/>
+      <c r="A35" s="92"/>
       <c r="B35" s="24" t="s">
         <v>14</v>
       </c>
@@ -2411,13 +2423,13 @@
         <v>11</v>
       </c>
       <c r="D35" s="38"/>
-      <c r="E35" s="89"/>
+      <c r="E35" s="71"/>
       <c r="F35" s="63" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="84"/>
+      <c r="A36" s="92"/>
       <c r="B36" s="24" t="s">
         <v>15</v>
       </c>
@@ -2425,13 +2437,13 @@
         <v>16</v>
       </c>
       <c r="D36" s="38"/>
-      <c r="E36" s="89"/>
+      <c r="E36" s="71"/>
       <c r="F36" s="54" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="84"/>
+      <c r="A37" s="92"/>
       <c r="B37" s="24" t="s">
         <v>17</v>
       </c>
@@ -2439,13 +2451,13 @@
         <v>18</v>
       </c>
       <c r="D37" s="38"/>
-      <c r="E37" s="89"/>
+      <c r="E37" s="71"/>
       <c r="F37" s="54" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="84"/>
+      <c r="A38" s="92"/>
       <c r="B38" s="24" t="s">
         <v>170</v>
       </c>
@@ -2453,13 +2465,13 @@
         <v>19</v>
       </c>
       <c r="D38" s="43"/>
-      <c r="E38" s="89"/>
+      <c r="E38" s="71"/>
       <c r="F38" s="63" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="84"/>
+      <c r="A39" s="92"/>
       <c r="B39" s="24" t="s">
         <v>171</v>
       </c>
@@ -2467,13 +2479,13 @@
         <v>20</v>
       </c>
       <c r="D39" s="38"/>
-      <c r="E39" s="89"/>
+      <c r="E39" s="71"/>
       <c r="F39" s="54" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="84"/>
+      <c r="A40" s="92"/>
       <c r="B40" s="24" t="s">
         <v>21</v>
       </c>
@@ -2481,13 +2493,13 @@
         <v>97</v>
       </c>
       <c r="D40" s="38"/>
-      <c r="E40" s="89"/>
+      <c r="E40" s="71"/>
       <c r="F40" s="63" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="84"/>
+      <c r="A41" s="92"/>
       <c r="B41" s="24" t="s">
         <v>22</v>
       </c>
@@ -2495,13 +2507,13 @@
         <v>23</v>
       </c>
       <c r="D41" s="38"/>
-      <c r="E41" s="89"/>
+      <c r="E41" s="71"/>
       <c r="F41" s="54" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="84"/>
+      <c r="A42" s="92"/>
       <c r="B42" s="24" t="s">
         <v>24</v>
       </c>
@@ -2509,13 +2521,13 @@
         <v>25</v>
       </c>
       <c r="D42" s="38"/>
-      <c r="E42" s="89"/>
+      <c r="E42" s="71"/>
       <c r="F42" s="64" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="84"/>
+      <c r="A43" s="92"/>
       <c r="B43" s="24" t="s">
         <v>26</v>
       </c>
@@ -2523,13 +2535,13 @@
         <v>27</v>
       </c>
       <c r="D43" s="38"/>
-      <c r="E43" s="89"/>
+      <c r="E43" s="71"/>
       <c r="F43" s="54" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="84"/>
+      <c r="A44" s="92"/>
       <c r="B44" s="24" t="s">
         <v>28</v>
       </c>
@@ -2537,13 +2549,13 @@
         <v>29</v>
       </c>
       <c r="D44" s="38"/>
-      <c r="E44" s="89"/>
+      <c r="E44" s="71"/>
       <c r="F44" s="54" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="84"/>
+      <c r="A45" s="92"/>
       <c r="B45" s="24" t="s">
         <v>30</v>
       </c>
@@ -2551,13 +2563,13 @@
         <v>98</v>
       </c>
       <c r="D45" s="40"/>
-      <c r="E45" s="89"/>
+      <c r="E45" s="71"/>
       <c r="F45" s="54" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="84"/>
+      <c r="A46" s="92"/>
       <c r="B46" s="24" t="s">
         <v>31</v>
       </c>
@@ -2565,13 +2577,13 @@
         <v>98</v>
       </c>
       <c r="D46" s="40"/>
-      <c r="E46" s="89"/>
+      <c r="E46" s="71"/>
       <c r="F46" s="54" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="84"/>
+      <c r="A47" s="92"/>
       <c r="B47" s="24" t="s">
         <v>32</v>
       </c>
@@ -2579,13 +2591,13 @@
         <v>98</v>
       </c>
       <c r="D47" s="40"/>
-      <c r="E47" s="89"/>
+      <c r="E47" s="71"/>
       <c r="F47" s="54" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="84"/>
+      <c r="A48" s="92"/>
       <c r="B48" s="24" t="s">
         <v>120</v>
       </c>
@@ -2593,25 +2605,25 @@
         <v>99</v>
       </c>
       <c r="D48" s="38"/>
-      <c r="E48" s="89"/>
+      <c r="E48" s="71"/>
       <c r="F48" s="54" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="84"/>
+      <c r="A49" s="92"/>
       <c r="B49" s="24" t="s">
         <v>122</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="38"/>
-      <c r="E49" s="89"/>
+      <c r="E49" s="71"/>
       <c r="F49" s="62" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="84"/>
+      <c r="A50" s="92"/>
       <c r="B50" s="29" t="s">
         <v>121</v>
       </c>
@@ -2619,13 +2631,13 @@
         <v>100</v>
       </c>
       <c r="D50" s="41"/>
-      <c r="E50" s="91"/>
+      <c r="E50" s="73"/>
       <c r="F50" s="55" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="81" t="s">
+      <c r="A51" s="89" t="s">
         <v>33</v>
       </c>
       <c r="B51" s="24" t="s">
@@ -2635,13 +2647,13 @@
         <v>34</v>
       </c>
       <c r="D51" s="38"/>
-      <c r="E51" s="89"/>
+      <c r="E51" s="71"/>
       <c r="F51" s="54" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="82"/>
+      <c r="A52" s="90"/>
       <c r="B52" s="29" t="s">
         <v>35</v>
       </c>
@@ -2649,7 +2661,7 @@
         <v>34</v>
       </c>
       <c r="D52" s="41"/>
-      <c r="E52" s="89"/>
+      <c r="E52" s="71"/>
       <c r="F52" s="59"/>
     </row>
     <row r="53" spans="1:6" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2663,13 +2675,13 @@
         <v>37</v>
       </c>
       <c r="D53" s="44"/>
-      <c r="E53" s="94"/>
+      <c r="E53" s="76"/>
       <c r="F53" s="55" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="81" t="s">
+      <c r="A54" s="89" t="s">
         <v>38</v>
       </c>
       <c r="B54" s="24" t="s">
@@ -2679,13 +2691,13 @@
         <v>0</v>
       </c>
       <c r="D54" s="38"/>
-      <c r="E54" s="89"/>
+      <c r="E54" s="71"/>
       <c r="F54" s="54" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="83"/>
+      <c r="A55" s="91"/>
       <c r="B55" s="24" t="s">
         <v>39</v>
       </c>
@@ -2693,13 +2705,13 @@
         <v>0</v>
       </c>
       <c r="D55" s="38"/>
-      <c r="E55" s="89"/>
+      <c r="E55" s="71"/>
       <c r="F55" s="35">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="83"/>
+      <c r="A56" s="91"/>
       <c r="B56" s="24" t="s">
         <v>40</v>
       </c>
@@ -2707,13 +2719,13 @@
         <v>1</v>
       </c>
       <c r="D56" s="38"/>
-      <c r="E56" s="89"/>
+      <c r="E56" s="71"/>
       <c r="F56" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="83"/>
+      <c r="A57" s="91"/>
       <c r="B57" s="24" t="s">
         <v>41</v>
       </c>
@@ -2721,13 +2733,13 @@
         <v>255</v>
       </c>
       <c r="D57" s="38"/>
-      <c r="E57" s="89"/>
+      <c r="E57" s="71"/>
       <c r="F57" s="35">
         <v>255</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="83"/>
+      <c r="A58" s="91"/>
       <c r="B58" s="23" t="s">
         <v>42</v>
       </c>
@@ -2735,13 +2747,13 @@
         <v>63</v>
       </c>
       <c r="D58" s="38"/>
-      <c r="E58" s="89"/>
+      <c r="E58" s="71"/>
       <c r="F58" s="35">
         <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="83"/>
+      <c r="A59" s="91"/>
       <c r="B59" s="24" t="s">
         <v>43</v>
       </c>
@@ -2749,13 +2761,13 @@
         <v>193</v>
       </c>
       <c r="D59" s="38"/>
-      <c r="E59" s="89"/>
+      <c r="E59" s="71"/>
       <c r="F59" s="35">
         <v>193</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="83"/>
+      <c r="A60" s="91"/>
       <c r="B60" s="24" t="s">
         <v>44</v>
       </c>
@@ -2763,13 +2775,13 @@
         <v>255</v>
       </c>
       <c r="D60" s="38"/>
-      <c r="E60" s="89"/>
+      <c r="E60" s="71"/>
       <c r="F60" s="35">
         <v>255</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="83"/>
+      <c r="A61" s="91"/>
       <c r="B61" s="24" t="s">
         <v>45</v>
       </c>
@@ -2777,13 +2789,13 @@
         <v>255</v>
       </c>
       <c r="D61" s="38"/>
-      <c r="E61" s="89"/>
+      <c r="E61" s="71"/>
       <c r="F61" s="35">
         <v>255</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="83"/>
+      <c r="A62" s="91"/>
       <c r="B62" s="24" t="s">
         <v>46</v>
       </c>
@@ -2791,13 +2803,13 @@
         <v>255</v>
       </c>
       <c r="D62" s="38"/>
-      <c r="E62" s="89"/>
+      <c r="E62" s="71"/>
       <c r="F62" s="60" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="83"/>
+      <c r="A63" s="91"/>
       <c r="B63" s="24" t="s">
         <v>47</v>
       </c>
@@ -2805,13 +2817,13 @@
         <v>101</v>
       </c>
       <c r="D63" s="45"/>
-      <c r="E63" s="89"/>
+      <c r="E63" s="71"/>
       <c r="F63" s="54" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="82"/>
+      <c r="A64" s="90"/>
       <c r="B64" s="29" t="s">
         <v>48</v>
       </c>
@@ -2819,13 +2831,13 @@
         <v>255</v>
       </c>
       <c r="D64" s="41"/>
-      <c r="E64" s="91"/>
+      <c r="E64" s="73"/>
       <c r="F64" s="61" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="85" t="s">
+      <c r="A65" s="93" t="s">
         <v>49</v>
       </c>
       <c r="B65" s="24" t="s">
@@ -2835,37 +2847,37 @@
         <v>51</v>
       </c>
       <c r="D65" s="38"/>
-      <c r="E65" s="89"/>
+      <c r="E65" s="71"/>
       <c r="F65" s="60" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="84"/>
+      <c r="A66" s="92"/>
       <c r="B66" s="24" t="s">
         <v>128</v>
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="38"/>
-      <c r="E66" s="89"/>
+      <c r="E66" s="71"/>
       <c r="F66" s="60" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="84"/>
+      <c r="A67" s="92"/>
       <c r="B67" s="24" t="s">
         <v>129</v>
       </c>
       <c r="C67" s="10"/>
       <c r="D67" s="38"/>
-      <c r="E67" s="89"/>
+      <c r="E67" s="71"/>
       <c r="F67" s="60" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="84"/>
+      <c r="A68" s="92"/>
       <c r="B68" s="24" t="s">
         <v>52</v>
       </c>
@@ -2873,13 +2885,13 @@
         <v>53</v>
       </c>
       <c r="D68" s="38"/>
-      <c r="E68" s="89"/>
+      <c r="E68" s="71"/>
       <c r="F68" s="58" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="84"/>
+      <c r="A69" s="92"/>
       <c r="B69" s="24" t="s">
         <v>184</v>
       </c>
@@ -2887,13 +2899,13 @@
         <v>54</v>
       </c>
       <c r="D69" s="38"/>
-      <c r="E69" s="89"/>
+      <c r="E69" s="71"/>
       <c r="F69" s="60" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="84"/>
+      <c r="A70" s="92"/>
       <c r="B70" s="24" t="s">
         <v>49</v>
       </c>
@@ -2901,13 +2913,13 @@
         <v>55</v>
       </c>
       <c r="D70" s="38"/>
-      <c r="E70" s="89"/>
+      <c r="E70" s="71"/>
       <c r="F70" s="54" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="84"/>
+      <c r="A71" s="92"/>
       <c r="B71" s="24" t="s">
         <v>56</v>
       </c>
@@ -2915,13 +2927,13 @@
         <v>53</v>
       </c>
       <c r="D71" s="38"/>
-      <c r="E71" s="89"/>
+      <c r="E71" s="71"/>
       <c r="F71" s="58" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="84"/>
+      <c r="A72" s="92"/>
       <c r="B72" s="24" t="s">
         <v>57</v>
       </c>
@@ -2929,37 +2941,37 @@
         <v>53</v>
       </c>
       <c r="D72" s="38"/>
-      <c r="E72" s="89"/>
+      <c r="E72" s="71"/>
       <c r="F72" s="58" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="84"/>
+      <c r="A73" s="92"/>
       <c r="B73" s="24" t="s">
         <v>189</v>
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="38"/>
-      <c r="E73" s="89"/>
+      <c r="E73" s="71"/>
       <c r="F73" s="65" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="84"/>
+      <c r="A74" s="92"/>
       <c r="B74" s="24" t="s">
         <v>190</v>
       </c>
       <c r="C74" s="10"/>
       <c r="D74" s="38"/>
-      <c r="E74" s="89"/>
+      <c r="E74" s="71"/>
       <c r="F74" s="65" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="84"/>
+      <c r="A75" s="92"/>
       <c r="B75" s="24" t="s">
         <v>58</v>
       </c>
@@ -2967,37 +2979,37 @@
         <v>59</v>
       </c>
       <c r="D75" s="42"/>
-      <c r="E75" s="89"/>
+      <c r="E75" s="71"/>
       <c r="F75" s="65" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="84"/>
+      <c r="A76" s="92"/>
       <c r="B76" s="24" t="s">
         <v>60</v>
       </c>
       <c r="C76" s="13"/>
       <c r="D76" s="40"/>
-      <c r="E76" s="95"/>
+      <c r="E76" s="77"/>
       <c r="F76" s="54" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="86"/>
+      <c r="A77" s="94"/>
       <c r="B77" s="29" t="s">
         <v>61</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="46"/>
-      <c r="E77" s="91"/>
+      <c r="E77" s="73"/>
       <c r="F77" s="55" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="81" t="s">
+      <c r="A78" s="89" t="s">
         <v>62</v>
       </c>
       <c r="B78" s="24" t="s">
@@ -3007,13 +3019,13 @@
         <v>63</v>
       </c>
       <c r="D78" s="38"/>
-      <c r="E78" s="89"/>
+      <c r="E78" s="71"/>
       <c r="F78" s="65" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="87"/>
+      <c r="A79" s="95"/>
       <c r="B79" s="23" t="s">
         <v>109</v>
       </c>
@@ -3021,13 +3033,13 @@
         <v>64</v>
       </c>
       <c r="D79" s="38"/>
-      <c r="E79" s="89"/>
+      <c r="E79" s="71"/>
       <c r="F79" s="58" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="87"/>
+      <c r="A80" s="95"/>
       <c r="B80" s="24" t="s">
         <v>65</v>
       </c>
@@ -3035,61 +3047,61 @@
         <v>66</v>
       </c>
       <c r="D80" s="38"/>
-      <c r="E80" s="89"/>
+      <c r="E80" s="71"/>
       <c r="F80" s="58" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="87"/>
+      <c r="A81" s="95"/>
       <c r="B81" s="24" t="s">
         <v>67</v>
       </c>
       <c r="C81" s="10"/>
       <c r="D81" s="38"/>
-      <c r="E81" s="89"/>
+      <c r="E81" s="71"/>
       <c r="F81" s="54" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="87"/>
+      <c r="A82" s="95"/>
       <c r="B82" s="23" t="s">
         <v>110</v>
       </c>
       <c r="C82" s="10"/>
       <c r="D82" s="38"/>
-      <c r="E82" s="89"/>
+      <c r="E82" s="71"/>
       <c r="F82" s="58" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="87"/>
+      <c r="A83" s="95"/>
       <c r="B83" s="24" t="s">
         <v>68</v>
       </c>
       <c r="C83" s="10"/>
       <c r="D83" s="38"/>
-      <c r="E83" s="89"/>
+      <c r="E83" s="71"/>
       <c r="F83" s="58" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="87"/>
+      <c r="A84" s="95"/>
       <c r="B84" s="29" t="s">
         <v>69</v>
       </c>
       <c r="C84" s="10"/>
       <c r="D84" s="41"/>
-      <c r="E84" s="91"/>
+      <c r="E84" s="73"/>
       <c r="F84" s="59" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="81" t="s">
+      <c r="A85" s="89" t="s">
         <v>70</v>
       </c>
       <c r="B85" s="24" t="s">
@@ -3099,13 +3111,13 @@
         <v>71</v>
       </c>
       <c r="D85" s="38"/>
-      <c r="E85" s="89"/>
+      <c r="E85" s="71"/>
       <c r="F85" s="66" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="87"/>
+      <c r="A86" s="95"/>
       <c r="B86" s="23" t="s">
         <v>116</v>
       </c>
@@ -3113,13 +3125,13 @@
         <v>72</v>
       </c>
       <c r="D86" s="38"/>
-      <c r="E86" s="89"/>
+      <c r="E86" s="71"/>
       <c r="F86" s="66" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="87"/>
+      <c r="A87" s="95"/>
       <c r="B87" s="24" t="s">
         <v>70</v>
       </c>
@@ -3127,37 +3139,37 @@
         <v>73</v>
       </c>
       <c r="D87" s="38"/>
-      <c r="E87" s="89"/>
+      <c r="E87" s="71"/>
       <c r="F87" s="66" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="87"/>
+      <c r="A88" s="95"/>
       <c r="B88" s="23" t="s">
         <v>102</v>
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="38"/>
-      <c r="E88" s="89"/>
+      <c r="E88" s="71"/>
       <c r="F88" s="54" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="87"/>
+      <c r="A89" s="95"/>
       <c r="B89" s="24" t="s">
         <v>130</v>
       </c>
       <c r="C89" s="10"/>
       <c r="D89" s="38"/>
-      <c r="E89" s="89"/>
+      <c r="E89" s="71"/>
       <c r="F89" s="66" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="87"/>
+      <c r="A90" s="95"/>
       <c r="B90" s="24" t="s">
         <v>74</v>
       </c>
@@ -3165,25 +3177,25 @@
         <v>75</v>
       </c>
       <c r="D90" s="38"/>
-      <c r="E90" s="89"/>
+      <c r="E90" s="71"/>
       <c r="F90" s="66" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="87"/>
+      <c r="A91" s="95"/>
       <c r="B91" s="24" t="s">
         <v>199</v>
       </c>
       <c r="C91" s="10"/>
       <c r="D91" s="38"/>
-      <c r="E91" s="89"/>
+      <c r="E91" s="71"/>
       <c r="F91" s="58" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="87"/>
+      <c r="A92" s="95"/>
       <c r="B92" s="24" t="s">
         <v>115</v>
       </c>
@@ -3191,7 +3203,7 @@
         <v>76</v>
       </c>
       <c r="D92" s="38"/>
-      <c r="E92" s="96" t="s">
+      <c r="E92" s="78" t="s">
         <v>275</v>
       </c>
       <c r="F92" s="58" t="s">
@@ -3199,7 +3211,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="88"/>
+      <c r="A93" s="96"/>
       <c r="B93" s="32" t="s">
         <v>117</v>
       </c>
@@ -3207,7 +3219,7 @@
         <v>77</v>
       </c>
       <c r="D93" s="41"/>
-      <c r="E93" s="91"/>
+      <c r="E93" s="73"/>
       <c r="F93" s="55" t="s">
         <v>252</v>
       </c>
@@ -3225,7 +3237,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="75" t="s">
+      <c r="A95" s="83" t="s">
         <v>78</v>
       </c>
       <c r="B95" s="24" t="s">
@@ -3241,7 +3253,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="75"/>
+      <c r="A96" s="83"/>
       <c r="B96" s="24" t="s">
         <v>141</v>
       </c>
@@ -3255,7 +3267,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="75"/>
+      <c r="A97" s="83"/>
       <c r="B97" s="24" t="s">
         <v>134</v>
       </c>
@@ -3269,7 +3281,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="75"/>
+      <c r="A98" s="83"/>
       <c r="B98" s="24" t="s">
         <v>220</v>
       </c>
@@ -3281,7 +3293,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="75"/>
+      <c r="A99" s="83"/>
       <c r="B99" s="24" t="s">
         <v>139</v>
       </c>
@@ -3293,7 +3305,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="75"/>
+      <c r="A100" s="83"/>
       <c r="B100" s="24" t="s">
         <v>140</v>
       </c>
@@ -3305,7 +3317,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="75"/>
+      <c r="A101" s="83"/>
       <c r="B101" s="24" t="s">
         <v>135</v>
       </c>
@@ -3319,7 +3331,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="75"/>
+      <c r="A102" s="83"/>
       <c r="B102" s="24" t="s">
         <v>136</v>
       </c>
@@ -3333,7 +3345,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="75"/>
+      <c r="A103" s="83"/>
       <c r="B103" s="24" t="s">
         <v>137</v>
       </c>
@@ -3347,7 +3359,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="76"/>
+      <c r="A104" s="84"/>
       <c r="B104" s="29" t="s">
         <v>138</v>
       </c>
@@ -3361,7 +3373,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="74" t="s">
+      <c r="A105" s="82" t="s">
         <v>148</v>
       </c>
       <c r="B105" s="24" t="s">
@@ -3371,13 +3383,13 @@
         <v>86</v>
       </c>
       <c r="D105" s="38"/>
-      <c r="E105" s="89"/>
+      <c r="E105" s="71"/>
       <c r="F105" s="65" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="75"/>
+      <c r="A106" s="83"/>
       <c r="B106" s="24" t="s">
         <v>127</v>
       </c>
@@ -3385,13 +3397,13 @@
         <v>87</v>
       </c>
       <c r="D106" s="42"/>
-      <c r="E106" s="89"/>
+      <c r="E106" s="71"/>
       <c r="F106" s="65" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="75"/>
+      <c r="A107" s="83"/>
       <c r="B107" s="24" t="s">
         <v>142</v>
       </c>
@@ -3399,227 +3411,250 @@
         <v>88</v>
       </c>
       <c r="D107" s="47"/>
-      <c r="E107" s="89"/>
+      <c r="E107" s="71"/>
       <c r="F107" s="65" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="75"/>
+      <c r="A108" s="83"/>
       <c r="B108" s="24" t="s">
         <v>143</v>
       </c>
       <c r="C108" s="16"/>
       <c r="D108" s="47"/>
-      <c r="E108" s="89"/>
+      <c r="E108" s="71"/>
       <c r="F108" s="65" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="75"/>
+      <c r="A109" s="83"/>
       <c r="B109" s="24" t="s">
         <v>144</v>
       </c>
       <c r="C109" s="16"/>
       <c r="D109" s="47"/>
-      <c r="E109" s="89"/>
+      <c r="E109" s="71"/>
       <c r="F109" s="58" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="75"/>
-      <c r="B110" s="28" t="s">
-        <v>249</v>
+      <c r="A110" s="83"/>
+      <c r="B110" s="24" t="s">
+        <v>277</v>
       </c>
       <c r="C110" s="16"/>
       <c r="D110" s="47"/>
-      <c r="E110" s="89"/>
-      <c r="F110" s="65" t="s">
+      <c r="E110" s="71"/>
+      <c r="F110" s="66" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="83"/>
+      <c r="B111" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="C111" s="16"/>
+      <c r="D111" s="47"/>
+      <c r="E111" s="71"/>
+      <c r="F111" s="65" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="76"/>
-      <c r="B111" s="33" t="s">
+    <row r="112" spans="1:6" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="84"/>
+      <c r="B112" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="C111" s="7"/>
-      <c r="D111" s="48"/>
-      <c r="E111" s="91"/>
-      <c r="F111" s="55" t="s">
+      <c r="C112" s="7"/>
+      <c r="D112" s="48"/>
+      <c r="E112" s="73"/>
+      <c r="F112" s="55" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="74" t="s">
+    <row r="113" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="82" t="s">
         <v>149</v>
       </c>
-      <c r="B112" s="24" t="s">
+      <c r="B113" s="24" t="s">
         <v>145</v>
-      </c>
-      <c r="C112" s="16"/>
-      <c r="D112" s="47"/>
-      <c r="E112" s="89"/>
-      <c r="F112" s="65" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="75"/>
-      <c r="B113" s="24" t="s">
-        <v>147</v>
       </c>
       <c r="C113" s="16"/>
       <c r="D113" s="47"/>
-      <c r="E113" s="89"/>
+      <c r="E113" s="71"/>
       <c r="F113" s="65" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="75"/>
+      <c r="A114" s="83"/>
       <c r="B114" s="24" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C114" s="16"/>
       <c r="D114" s="47"/>
-      <c r="E114" s="89"/>
+      <c r="E114" s="71"/>
       <c r="F114" s="65" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="83"/>
+      <c r="B115" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C115" s="16"/>
+      <c r="D115" s="47"/>
+      <c r="E115" s="71"/>
+      <c r="F115" s="65" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="75"/>
-      <c r="B115" s="24" t="s">
+    <row r="116" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="83"/>
+      <c r="B116" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="C115" s="14" t="s">
+      <c r="C116" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="D115" s="42"/>
-      <c r="E115" s="89"/>
-      <c r="F115" s="65" t="s">
+      <c r="D116" s="42"/>
+      <c r="E116" s="71"/>
+      <c r="F116" s="65" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="75"/>
-      <c r="B116" s="24" t="s">
+    <row r="117" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="83"/>
+      <c r="B117" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="C116" s="14" t="s">
+      <c r="C117" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D116" s="42"/>
-      <c r="E116" s="89"/>
-      <c r="F116" s="65" t="s">
+      <c r="D117" s="42"/>
+      <c r="E117" s="71"/>
+      <c r="F117" s="65" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="75"/>
-      <c r="B117" s="34" t="s">
+    <row r="118" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="83"/>
+      <c r="B118" s="34" t="s">
         <v>217</v>
-      </c>
-      <c r="C117" s="13"/>
-      <c r="D117" s="40"/>
-      <c r="E117" s="89"/>
-      <c r="F117" s="54" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="75"/>
-      <c r="B118" s="24" t="s">
-        <v>218</v>
       </c>
       <c r="C118" s="13"/>
       <c r="D118" s="40"/>
-      <c r="E118" s="89"/>
-      <c r="F118" s="65" t="s">
+      <c r="E118" s="71"/>
+      <c r="F118" s="54" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="83"/>
+      <c r="B119" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="C119" s="13"/>
+      <c r="D119" s="40"/>
+      <c r="E119" s="71"/>
+      <c r="F119" s="65" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="76"/>
-      <c r="B119" s="29" t="s">
+    <row r="120" spans="1:6" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="84"/>
+      <c r="B120" s="29" t="s">
         <v>219</v>
       </c>
-      <c r="C119" s="4"/>
-      <c r="D119" s="46"/>
-      <c r="E119" s="91"/>
-      <c r="F119" s="55" t="s">
+      <c r="C120" s="4"/>
+      <c r="D120" s="46"/>
+      <c r="E120" s="73"/>
+      <c r="F120" s="55" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="71" t="s">
+    <row r="121" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="79" t="s">
         <v>242</v>
       </c>
-      <c r="B120" s="35" t="s">
+      <c r="B121" s="35" t="s">
         <v>258</v>
       </c>
-      <c r="D120" s="18"/>
-      <c r="E120" s="89"/>
-      <c r="F120" s="54" t="s">
+      <c r="D121" s="18"/>
+      <c r="E121" s="71"/>
+      <c r="F121" s="54" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="72"/>
-      <c r="B121" s="35" t="s">
+    <row r="122" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="80"/>
+      <c r="B122" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="D121" s="18"/>
-      <c r="E121" s="89"/>
-      <c r="F121" s="62"/>
-    </row>
-    <row r="122" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="72"/>
-      <c r="B122" s="35" t="s">
+      <c r="D122" s="18"/>
+      <c r="E122" s="71"/>
+      <c r="F122" s="62"/>
+    </row>
+    <row r="123" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="80"/>
+      <c r="B123" s="35" t="s">
         <v>260</v>
       </c>
-      <c r="D122" s="18"/>
-      <c r="E122" s="89"/>
-      <c r="F122" s="54" t="s">
+      <c r="D123" s="18"/>
+      <c r="E123" s="71"/>
+      <c r="F123" s="54" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="72"/>
-      <c r="B123" s="35" t="s">
+    <row r="124" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="80"/>
+      <c r="B124" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="D123" s="18"/>
-      <c r="E123" s="89"/>
-      <c r="F123" s="62"/>
-    </row>
-    <row r="124" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="72"/>
-      <c r="B124" s="35" t="s">
+      <c r="D124" s="18"/>
+      <c r="E124" s="71"/>
+      <c r="F124" s="62"/>
+    </row>
+    <row r="125" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="80"/>
+      <c r="B125" s="60" t="s">
+        <v>279</v>
+      </c>
+      <c r="D125" s="18"/>
+      <c r="E125" s="71"/>
+      <c r="F125" s="54" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="80"/>
+      <c r="B126" s="35" t="s">
         <v>262</v>
       </c>
-      <c r="D124" s="18"/>
-      <c r="E124" s="89"/>
-      <c r="F124" s="62"/>
-    </row>
-    <row r="125" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="73"/>
-      <c r="B125" s="36" t="s">
+      <c r="D126" s="18"/>
+      <c r="E126" s="71"/>
+      <c r="F126" s="62"/>
+    </row>
+    <row r="127" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="81"/>
+      <c r="B127" s="36" t="s">
         <v>263</v>
       </c>
-      <c r="C125" s="9"/>
-      <c r="D125" s="49"/>
-      <c r="E125" s="91"/>
-      <c r="F125" s="70"/>
+      <c r="C127" s="9"/>
+      <c r="D127" s="49"/>
+      <c r="E127" s="73"/>
+      <c r="F127" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A120:A125"/>
-    <mergeCell ref="A105:A111"/>
-    <mergeCell ref="A112:A119"/>
+    <mergeCell ref="A121:A127"/>
+    <mergeCell ref="A105:A112"/>
+    <mergeCell ref="A113:A120"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A54:A64"/>

</xml_diff>